<commit_message>
Updated user mode vplan with link2cov
Signed-off-by: Marton Teilgard <mateilga@silabs.com>
</commit_message>
<xml_diff>
--- a/cv32e40s/docs/VerifPlans/Simulation/interrupts/CV32E40SX_CLIC.xlsx
+++ b/cv32e40s/docs/VerifPlans/Simulation/interrupts/CV32E40SX_CLIC.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ropeders\Documents\group_vplans\clic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\openhw\core-v-verif_40s\cv32e40s\docs\VerifPlans\Simulation\interrupts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4636D7E2-2280-40F0-8D1F-683A503D101F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E62560B-BC24-4F97-A15A-1137DFC6130C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="High-level Feature" sheetId="1" r:id="rId1"/>
     <sheet name="DONOTDELETE" sheetId="2" r:id="rId2"/>
     <sheet name="References" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -59,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="383">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -2599,12 +2598,26 @@
   <si>
     <t xml:space="preserve"> ---- END ----</t>
   </si>
+  <si>
+    <t>A: uvmt_cv32e40s_tb.dut_wrap.cv32e40s_wrapper_i.core_i.clic_assert_i.gen_clic_assertions.a_mret_pc_intended,
+[clic_assert].a_mret_pc_not_vectored, 
+[clic_assert].a_mret_mode_mpp, 
+[clic_assert].a_mret_mil_mpil, 
+[clic_assert].a_mret_mil_mpil_intended, 
+[clic_assert].a_mret_mie_mpie</t>
+  </si>
+  <si>
+    <t>A: uvmt_cv32e40s_tb.dut_wrap.cv32e40s_wrapper_i.core_i.clic_assert_i.gen_clic_assertions.a_mret_umode_clear_mintthresh</t>
+  </si>
+  <si>
+    <t>A: uvmt_cv32e40s_tb.dut_wrap.cv32e40s_wrapper_i.core_i.clic_assert_i.gen_clic_assertions.a_dret_umode_clear_mintthresh</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2721,7 +2734,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2764,11 +2777,14 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2778,14 +2794,14 @@
   <dxfs count="2">
     <dxf>
       <font>
-        <color rgb="FFFF0000"/>
+        <b/>
+        <i/>
+        <color theme="8" tint="-0.24994659260841701"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i/>
-        <color theme="8" tint="-0.24994659260841701"/>
+        <color rgb="FFFF0000"/>
       </font>
     </dxf>
   </dxfs>
@@ -3193,26 +3209,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I152"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="I74" sqref="I74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="17" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="41.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.88671875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="54.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="41.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="74.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="30">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3241,7 +3257,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="57">
       <c r="A2" s="10" t="s">
         <v>30</v>
       </c>
@@ -3268,7 +3284,7 @@
       </c>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="57">
       <c r="A3" s="10" t="s">
         <v>30</v>
       </c>
@@ -3295,7 +3311,7 @@
       </c>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="28.5">
       <c r="A4" s="10" t="s">
         <v>36</v>
       </c>
@@ -3322,7 +3338,7 @@
       </c>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="42.75">
       <c r="A5" s="10" t="s">
         <v>39</v>
       </c>
@@ -3349,7 +3365,7 @@
       </c>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="42.75">
       <c r="A6" s="10" t="s">
         <v>36</v>
       </c>
@@ -3376,7 +3392,7 @@
       </c>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="57">
       <c r="A7" s="10" t="s">
         <v>36</v>
       </c>
@@ -3403,7 +3419,7 @@
       </c>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="28.5">
       <c r="A8" s="10" t="s">
         <v>36</v>
       </c>
@@ -3430,7 +3446,7 @@
       </c>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="28.5">
       <c r="A9" s="10" t="s">
         <v>36</v>
       </c>
@@ -3457,7 +3473,7 @@
       </c>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="28.5">
       <c r="A10" s="10" t="s">
         <v>36</v>
       </c>
@@ -3484,7 +3500,7 @@
       </c>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="1:9" ht="69" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="71.25">
       <c r="A11" s="10" t="s">
         <v>58</v>
       </c>
@@ -3511,7 +3527,7 @@
       </c>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="42.75">
       <c r="A12" s="10" t="s">
         <v>36</v>
       </c>
@@ -3538,7 +3554,7 @@
       </c>
       <c r="I12" s="5"/>
     </row>
-    <row r="13" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="28.5">
       <c r="A13" s="10" t="s">
         <v>58</v>
       </c>
@@ -3565,7 +3581,7 @@
       </c>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="28.5">
       <c r="A14" s="10" t="s">
         <v>58</v>
       </c>
@@ -3592,7 +3608,7 @@
       </c>
       <c r="I14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="42.75">
       <c r="A15" s="10" t="s">
         <v>58</v>
       </c>
@@ -3619,7 +3635,7 @@
       </c>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="28.5">
       <c r="A16" s="12" t="s">
         <v>58</v>
       </c>
@@ -3646,7 +3662,7 @@
       </c>
       <c r="I16" s="5"/>
     </row>
-    <row r="17" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="42.75">
       <c r="A17" s="12" t="s">
         <v>58</v>
       </c>
@@ -3673,7 +3689,7 @@
       </c>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="28.5">
       <c r="A18" s="10" t="s">
         <v>58</v>
       </c>
@@ -3700,7 +3716,7 @@
       </c>
       <c r="I18" s="5"/>
     </row>
-    <row r="19" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="57">
       <c r="A19" s="10" t="s">
         <v>85</v>
       </c>
@@ -3727,7 +3743,7 @@
       </c>
       <c r="I19" s="5"/>
     </row>
-    <row r="20" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="57">
       <c r="A20" s="10" t="s">
         <v>58</v>
       </c>
@@ -3754,7 +3770,7 @@
       </c>
       <c r="I20" s="5"/>
     </row>
-    <row r="21" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="28.5">
       <c r="A21" s="10" t="s">
         <v>30</v>
       </c>
@@ -3781,7 +3797,7 @@
       </c>
       <c r="I21" s="5"/>
     </row>
-    <row r="22" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="28.5">
       <c r="A22" s="10" t="s">
         <v>30</v>
       </c>
@@ -3808,7 +3824,7 @@
       </c>
       <c r="I22" s="5"/>
     </row>
-    <row r="23" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="28.5">
       <c r="A23" s="10" t="s">
         <v>30</v>
       </c>
@@ -3835,7 +3851,7 @@
       </c>
       <c r="I23" s="5"/>
     </row>
-    <row r="24" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="28.5">
       <c r="A24" s="10" t="s">
         <v>30</v>
       </c>
@@ -3862,7 +3878,7 @@
       </c>
       <c r="I24" s="5"/>
     </row>
-    <row r="25" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="28.5">
       <c r="A25" s="10" t="s">
         <v>30</v>
       </c>
@@ -3889,7 +3905,7 @@
       </c>
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="28.5">
       <c r="A26" s="10" t="s">
         <v>30</v>
       </c>
@@ -3916,7 +3932,7 @@
       </c>
       <c r="I26" s="5"/>
     </row>
-    <row r="27" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="28.5">
       <c r="A27" s="10" t="s">
         <v>30</v>
       </c>
@@ -3943,7 +3959,7 @@
       </c>
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="28.5">
       <c r="A28" s="10" t="s">
         <v>30</v>
       </c>
@@ -3970,7 +3986,7 @@
       </c>
       <c r="I28" s="5"/>
     </row>
-    <row r="29" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="28.5">
       <c r="A29" s="10" t="s">
         <v>36</v>
       </c>
@@ -3997,7 +4013,7 @@
       </c>
       <c r="I29" s="5"/>
     </row>
-    <row r="30" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="28.5">
       <c r="A30" s="10" t="s">
         <v>36</v>
       </c>
@@ -4024,7 +4040,7 @@
       </c>
       <c r="I30" s="5"/>
     </row>
-    <row r="31" spans="1:9" ht="69" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="71.25">
       <c r="A31" s="10" t="s">
         <v>58</v>
       </c>
@@ -4051,7 +4067,7 @@
       </c>
       <c r="I31" s="5"/>
     </row>
-    <row r="32" spans="1:9" ht="220.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="228">
       <c r="A32" s="10" t="s">
         <v>30</v>
       </c>
@@ -4078,7 +4094,7 @@
       </c>
       <c r="I32" s="5"/>
     </row>
-    <row r="33" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="28.5">
       <c r="A33" s="10" t="s">
         <v>36</v>
       </c>
@@ -4105,7 +4121,7 @@
       </c>
       <c r="I33" s="5"/>
     </row>
-    <row r="34" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="42.75">
       <c r="A34" s="10" t="s">
         <v>30</v>
       </c>
@@ -4132,7 +4148,7 @@
       </c>
       <c r="I34" s="5"/>
     </row>
-    <row r="35" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="42.75">
       <c r="A35" s="10" t="s">
         <v>30</v>
       </c>
@@ -4159,7 +4175,7 @@
       </c>
       <c r="I35" s="5"/>
     </row>
-    <row r="36" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="28.5">
       <c r="A36" s="10" t="s">
         <v>39</v>
       </c>
@@ -4186,7 +4202,7 @@
       </c>
       <c r="I36" s="5"/>
     </row>
-    <row r="37" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="28.5">
       <c r="A37" s="10" t="s">
         <v>30</v>
       </c>
@@ -4213,7 +4229,7 @@
       </c>
       <c r="I37" s="5"/>
     </row>
-    <row r="38" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="28.5">
       <c r="A38" s="10" t="s">
         <v>30</v>
       </c>
@@ -4240,7 +4256,7 @@
       </c>
       <c r="I38" s="5"/>
     </row>
-    <row r="39" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="42.75">
       <c r="A39" s="10" t="s">
         <v>30</v>
       </c>
@@ -4267,7 +4283,7 @@
       </c>
       <c r="I39" s="5"/>
     </row>
-    <row r="40" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="42.75">
       <c r="A40" s="10" t="s">
         <v>30</v>
       </c>
@@ -4294,7 +4310,7 @@
       </c>
       <c r="I40" s="5"/>
     </row>
-    <row r="41" spans="1:9" ht="165.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="171">
       <c r="A41" s="10" t="s">
         <v>30</v>
       </c>
@@ -4321,7 +4337,7 @@
       </c>
       <c r="I41" s="5"/>
     </row>
-    <row r="42" spans="1:9" ht="220.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="213.75">
       <c r="A42" s="10" t="s">
         <v>30</v>
       </c>
@@ -4348,7 +4364,7 @@
       </c>
       <c r="I42" s="5"/>
     </row>
-    <row r="43" spans="1:9" ht="179.4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="185.25">
       <c r="A43" s="10" t="s">
         <v>30</v>
       </c>
@@ -4375,7 +4391,7 @@
       </c>
       <c r="I43" s="5"/>
     </row>
-    <row r="44" spans="1:9" ht="220.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="213.75">
       <c r="A44" s="10" t="s">
         <v>30</v>
       </c>
@@ -4402,7 +4418,7 @@
       </c>
       <c r="I44" s="5"/>
     </row>
-    <row r="45" spans="1:9" ht="193.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="199.5">
       <c r="A45" s="10" t="s">
         <v>30</v>
       </c>
@@ -4429,7 +4445,7 @@
       </c>
       <c r="I45" s="5"/>
     </row>
-    <row r="46" spans="1:9" ht="151.80000000000001" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="142.5">
       <c r="A46" s="10" t="s">
         <v>30</v>
       </c>
@@ -4456,7 +4472,7 @@
       </c>
       <c r="I46" s="5"/>
     </row>
-    <row r="47" spans="1:9" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="99.75">
       <c r="A47" s="10" t="s">
         <v>367</v>
       </c>
@@ -4483,7 +4499,7 @@
       </c>
       <c r="I47" s="5"/>
     </row>
-    <row r="48" spans="1:9" ht="225" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="225" customHeight="1">
       <c r="A48" s="10" t="s">
         <v>36</v>
       </c>
@@ -4510,7 +4526,7 @@
       </c>
       <c r="I48" s="5"/>
     </row>
-    <row r="49" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="28.5">
       <c r="A49" s="10" t="s">
         <v>30</v>
       </c>
@@ -4537,7 +4553,7 @@
       </c>
       <c r="I49" s="5"/>
     </row>
-    <row r="50" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="42.75">
       <c r="A50" s="10" t="s">
         <v>30</v>
       </c>
@@ -4564,7 +4580,7 @@
       </c>
       <c r="I50" s="5"/>
     </row>
-    <row r="51" spans="1:9" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="57">
       <c r="A51" s="10" t="s">
         <v>30</v>
       </c>
@@ -4591,7 +4607,7 @@
       </c>
       <c r="I51" s="5"/>
     </row>
-    <row r="52" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="57">
       <c r="A52" s="10" t="s">
         <v>58</v>
       </c>
@@ -4618,7 +4634,7 @@
       </c>
       <c r="I52" s="5"/>
     </row>
-    <row r="53" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="57">
       <c r="A53" s="10" t="s">
         <v>30</v>
       </c>
@@ -4645,7 +4661,7 @@
       </c>
       <c r="I53" s="5"/>
     </row>
-    <row r="54" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="28.5">
       <c r="A54" s="10" t="s">
         <v>30</v>
       </c>
@@ -4672,7 +4688,7 @@
       </c>
       <c r="I54" s="5"/>
     </row>
-    <row r="55" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="42.75">
       <c r="A55" s="10" t="s">
         <v>36</v>
       </c>
@@ -4699,7 +4715,7 @@
       </c>
       <c r="I55" s="5"/>
     </row>
-    <row r="56" spans="1:9" ht="69" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="71.25">
       <c r="A56" s="10" t="s">
         <v>30</v>
       </c>
@@ -4726,7 +4742,7 @@
       </c>
       <c r="I56" s="5"/>
     </row>
-    <row r="57" spans="1:9" ht="234.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="228">
       <c r="A57" s="10" t="s">
         <v>30</v>
       </c>
@@ -4753,7 +4769,7 @@
       </c>
       <c r="I57" s="5"/>
     </row>
-    <row r="58" spans="1:9" ht="138" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="128.25">
       <c r="A58" s="10" t="s">
         <v>30</v>
       </c>
@@ -4780,7 +4796,7 @@
       </c>
       <c r="I58" s="5"/>
     </row>
-    <row r="59" spans="1:9" ht="262.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="256.5">
       <c r="A59" s="10" t="s">
         <v>30</v>
       </c>
@@ -4807,7 +4823,7 @@
       </c>
       <c r="I59" s="5"/>
     </row>
-    <row r="60" spans="1:9" ht="248.4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="242.25">
       <c r="A60" s="10" t="s">
         <v>30</v>
       </c>
@@ -4834,7 +4850,7 @@
       </c>
       <c r="I60" s="5"/>
     </row>
-    <row r="61" spans="1:9" ht="262.2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="270.75">
       <c r="A61" s="10" t="s">
         <v>30</v>
       </c>
@@ -4861,7 +4877,7 @@
       </c>
       <c r="I61" s="5"/>
     </row>
-    <row r="62" spans="1:9" ht="248.4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" ht="256.5">
       <c r="A62" s="10" t="s">
         <v>30</v>
       </c>
@@ -4888,7 +4904,7 @@
       </c>
       <c r="I62" s="5"/>
     </row>
-    <row r="63" spans="1:9" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="114">
       <c r="A63" s="10" t="s">
         <v>30</v>
       </c>
@@ -4915,7 +4931,7 @@
       </c>
       <c r="I63" s="5"/>
     </row>
-    <row r="64" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="57.75">
       <c r="A64" s="10" t="s">
         <v>30</v>
       </c>
@@ -4942,7 +4958,7 @@
       </c>
       <c r="I64" s="5"/>
     </row>
-    <row r="65" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" ht="57.75">
       <c r="A65" s="10" t="s">
         <v>30</v>
       </c>
@@ -4969,7 +4985,7 @@
       </c>
       <c r="I65" s="5"/>
     </row>
-    <row r="66" spans="1:9" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" ht="129">
       <c r="A66" s="10" t="s">
         <v>30</v>
       </c>
@@ -4996,7 +5012,7 @@
       </c>
       <c r="I66" s="5"/>
     </row>
-    <row r="67" spans="1:9" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" ht="128.25">
       <c r="A67" s="10" t="s">
         <v>30</v>
       </c>
@@ -5023,7 +5039,7 @@
       </c>
       <c r="I67" s="5"/>
     </row>
-    <row r="68" spans="1:9" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" ht="114">
       <c r="A68" s="10" t="s">
         <v>30</v>
       </c>
@@ -5050,7 +5066,7 @@
       </c>
       <c r="I68" s="5"/>
     </row>
-    <row r="69" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" ht="42.75">
       <c r="A69" s="10" t="s">
         <v>30</v>
       </c>
@@ -5077,7 +5093,7 @@
       </c>
       <c r="I69" s="5"/>
     </row>
-    <row r="70" spans="1:9" ht="69" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" ht="71.25">
       <c r="A70" s="10" t="s">
         <v>36</v>
       </c>
@@ -5104,7 +5120,7 @@
       </c>
       <c r="I70" s="5"/>
     </row>
-    <row r="71" spans="1:9" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" ht="128.25">
       <c r="A71" s="10" t="s">
         <v>30</v>
       </c>
@@ -5129,9 +5145,9 @@
       <c r="H71" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I71" s="5"/>
-    </row>
-    <row r="72" spans="1:9" ht="124.2" x14ac:dyDescent="0.3">
+      <c r="I71" s="20"/>
+    </row>
+    <row r="72" spans="1:9" ht="128.25">
       <c r="A72" s="10" t="s">
         <v>30</v>
       </c>
@@ -5156,9 +5172,11 @@
       <c r="H72" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I72" s="5"/>
-    </row>
-    <row r="73" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="I72" s="20" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="57">
       <c r="A73" s="10" t="s">
         <v>369</v>
       </c>
@@ -5183,9 +5201,11 @@
       <c r="H73" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I73" s="5"/>
-    </row>
-    <row r="74" spans="1:9" ht="69" x14ac:dyDescent="0.3">
+      <c r="I73" s="5" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="71.25">
       <c r="A74" s="10" t="s">
         <v>369</v>
       </c>
@@ -5210,9 +5230,11 @@
       <c r="H74" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I74" s="5"/>
-    </row>
-    <row r="75" spans="1:9" ht="124.2" x14ac:dyDescent="0.3">
+      <c r="I74" s="5" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="114">
       <c r="A75" s="10" t="s">
         <v>30</v>
       </c>
@@ -5239,7 +5261,7 @@
       </c>
       <c r="I75" s="5"/>
     </row>
-    <row r="76" spans="1:9" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" ht="128.25">
       <c r="A76" s="10" t="s">
         <v>30</v>
       </c>
@@ -5266,7 +5288,7 @@
       </c>
       <c r="I76" s="5"/>
     </row>
-    <row r="77" spans="1:9" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" ht="114">
       <c r="A77" s="10" t="s">
         <v>30</v>
       </c>
@@ -5293,7 +5315,7 @@
       </c>
       <c r="I77" s="5"/>
     </row>
-    <row r="78" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" ht="28.5">
       <c r="A78" s="10" t="s">
         <v>30</v>
       </c>
@@ -5320,7 +5342,7 @@
       </c>
       <c r="I78" s="5"/>
     </row>
-    <row r="79" spans="1:9" ht="42" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" ht="29.25">
       <c r="A79" s="10" t="s">
         <v>36</v>
       </c>
@@ -5347,7 +5369,7 @@
       </c>
       <c r="I79" s="5"/>
     </row>
-    <row r="80" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" ht="28.5">
       <c r="A80" s="10" t="s">
         <v>36</v>
       </c>
@@ -5374,7 +5396,7 @@
       </c>
       <c r="I80" s="5"/>
     </row>
-    <row r="81" spans="1:9" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" ht="29.25">
       <c r="A81" s="10" t="s">
         <v>36</v>
       </c>
@@ -5401,7 +5423,7 @@
       </c>
       <c r="I81" s="5"/>
     </row>
-    <row r="82" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" ht="42.75">
       <c r="A82" s="10" t="s">
         <v>30</v>
       </c>
@@ -5428,7 +5450,7 @@
       </c>
       <c r="I82" s="5"/>
     </row>
-    <row r="83" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" ht="57.75">
       <c r="A83" s="10" t="s">
         <v>30</v>
       </c>
@@ -5455,7 +5477,7 @@
       </c>
       <c r="I83" s="5"/>
     </row>
-    <row r="84" spans="1:9" ht="69" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" ht="71.25">
       <c r="A84" s="10" t="s">
         <v>36</v>
       </c>
@@ -5482,7 +5504,7 @@
       </c>
       <c r="I84" s="5"/>
     </row>
-    <row r="85" spans="1:9" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" ht="71.25">
       <c r="A85" s="10" t="s">
         <v>36</v>
       </c>
@@ -5509,7 +5531,7 @@
       </c>
       <c r="I85" s="5"/>
     </row>
-    <row r="86" spans="1:9" ht="207" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" ht="213.75">
       <c r="A86" s="10" t="s">
         <v>36</v>
       </c>
@@ -5536,7 +5558,7 @@
       </c>
       <c r="I86" s="5"/>
     </row>
-    <row r="87" spans="1:9" ht="220.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" ht="228">
       <c r="A87" s="10" t="s">
         <v>36</v>
       </c>
@@ -5563,7 +5585,7 @@
       </c>
       <c r="I87" s="5"/>
     </row>
-    <row r="88" spans="1:9" ht="179.4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" ht="185.25">
       <c r="A88" s="10" t="s">
         <v>36</v>
       </c>
@@ -5590,7 +5612,7 @@
       </c>
       <c r="I88" s="5"/>
     </row>
-    <row r="89" spans="1:9" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" ht="128.25">
       <c r="A89" s="10" t="s">
         <v>36</v>
       </c>
@@ -5617,7 +5639,7 @@
       </c>
       <c r="I89" s="5"/>
     </row>
-    <row r="90" spans="1:9" ht="151.80000000000001" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" ht="156.75">
       <c r="A90" s="10" t="s">
         <v>36</v>
       </c>
@@ -5644,7 +5666,7 @@
       </c>
       <c r="I90" s="5"/>
     </row>
-    <row r="91" spans="1:9" ht="165.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" ht="171">
       <c r="A91" s="10" t="s">
         <v>36</v>
       </c>
@@ -5671,7 +5693,7 @@
       </c>
       <c r="I91" s="5"/>
     </row>
-    <row r="92" spans="1:9" ht="138" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" ht="142.5">
       <c r="A92" s="10" t="s">
         <v>36</v>
       </c>
@@ -5698,7 +5720,7 @@
       </c>
       <c r="I92" s="5"/>
     </row>
-    <row r="93" spans="1:9" ht="220.8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" ht="213.75">
       <c r="A93" s="10" t="s">
         <v>36</v>
       </c>
@@ -5725,7 +5747,7 @@
       </c>
       <c r="I93" s="5"/>
     </row>
-    <row r="94" spans="1:9" ht="220.8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" ht="228">
       <c r="A94" s="10" t="s">
         <v>36</v>
       </c>
@@ -5752,7 +5774,7 @@
       </c>
       <c r="I94" s="5"/>
     </row>
-    <row r="95" spans="1:9" ht="151.80000000000001" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" ht="156.75">
       <c r="A95" s="10" t="s">
         <v>36</v>
       </c>
@@ -5779,7 +5801,7 @@
       </c>
       <c r="I95" s="5"/>
     </row>
-    <row r="96" spans="1:9" ht="138" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" ht="142.5">
       <c r="A96" s="10" t="s">
         <v>36</v>
       </c>
@@ -5806,7 +5828,7 @@
       </c>
       <c r="I96" s="5"/>
     </row>
-    <row r="97" spans="1:9" ht="151.80000000000001" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" ht="156.75">
       <c r="A97" s="10" t="s">
         <v>36</v>
       </c>
@@ -5833,7 +5855,7 @@
       </c>
       <c r="I97" s="5"/>
     </row>
-    <row r="98" spans="1:9" ht="207" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" ht="213.75">
       <c r="A98" s="10" t="s">
         <v>36</v>
       </c>
@@ -5860,7 +5882,7 @@
       </c>
       <c r="I98" s="5"/>
     </row>
-    <row r="99" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" ht="29.25">
       <c r="A99" s="10" t="s">
         <v>39</v>
       </c>
@@ -5887,7 +5909,7 @@
       </c>
       <c r="I99" s="5"/>
     </row>
-    <row r="100" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" ht="29.25">
       <c r="A100" s="10" t="s">
         <v>39</v>
       </c>
@@ -5914,7 +5936,7 @@
       </c>
       <c r="I100" s="5"/>
     </row>
-    <row r="101" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" ht="29.25">
       <c r="A101" s="10" t="s">
         <v>39</v>
       </c>
@@ -5941,7 +5963,7 @@
       </c>
       <c r="I101" s="5"/>
     </row>
-    <row r="102" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" ht="29.25">
       <c r="A102" s="10" t="s">
         <v>39</v>
       </c>
@@ -5968,7 +5990,7 @@
       </c>
       <c r="I102" s="5"/>
     </row>
-    <row r="103" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" ht="29.25">
       <c r="A103" s="10" t="s">
         <v>39</v>
       </c>
@@ -5995,7 +6017,7 @@
       </c>
       <c r="I103" s="5"/>
     </row>
-    <row r="104" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" ht="29.25">
       <c r="A104" s="10" t="s">
         <v>39</v>
       </c>
@@ -6022,7 +6044,7 @@
       </c>
       <c r="I104" s="5"/>
     </row>
-    <row r="105" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" ht="29.25">
       <c r="A105" s="10" t="s">
         <v>39</v>
       </c>
@@ -6049,7 +6071,7 @@
       </c>
       <c r="I105" s="5"/>
     </row>
-    <row r="106" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" ht="29.25">
       <c r="A106" s="10" t="s">
         <v>39</v>
       </c>
@@ -6076,7 +6098,7 @@
       </c>
       <c r="I106" s="5"/>
     </row>
-    <row r="107" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" ht="29.25">
       <c r="A107" s="10" t="s">
         <v>39</v>
       </c>
@@ -6103,7 +6125,7 @@
       </c>
       <c r="I107" s="5"/>
     </row>
-    <row r="108" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" ht="29.25">
       <c r="A108" s="10" t="s">
         <v>39</v>
       </c>
@@ -6130,7 +6152,7 @@
       </c>
       <c r="I108" s="5"/>
     </row>
-    <row r="109" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" ht="29.25">
       <c r="A109" s="10" t="s">
         <v>39</v>
       </c>
@@ -6157,7 +6179,7 @@
       </c>
       <c r="I109" s="5"/>
     </row>
-    <row r="110" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" ht="29.25">
       <c r="A110" s="10" t="s">
         <v>39</v>
       </c>
@@ -6184,7 +6206,7 @@
       </c>
       <c r="I110" s="5"/>
     </row>
-    <row r="111" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" ht="29.25">
       <c r="A111" s="10" t="s">
         <v>39</v>
       </c>
@@ -6211,7 +6233,7 @@
       </c>
       <c r="I111" s="5"/>
     </row>
-    <row r="112" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" ht="29.25">
       <c r="A112" s="10" t="s">
         <v>39</v>
       </c>
@@ -6238,7 +6260,7 @@
       </c>
       <c r="I112" s="5"/>
     </row>
-    <row r="113" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" ht="29.25">
       <c r="A113" s="10" t="s">
         <v>39</v>
       </c>
@@ -6265,7 +6287,7 @@
       </c>
       <c r="I113" s="5"/>
     </row>
-    <row r="114" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" ht="29.25">
       <c r="A114" s="10" t="s">
         <v>39</v>
       </c>
@@ -6292,7 +6314,7 @@
       </c>
       <c r="I114" s="5"/>
     </row>
-    <row r="115" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" ht="29.25">
       <c r="A115" s="10" t="s">
         <v>39</v>
       </c>
@@ -6319,7 +6341,7 @@
       </c>
       <c r="I115" s="5"/>
     </row>
-    <row r="116" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" ht="29.25">
       <c r="A116" s="10" t="s">
         <v>39</v>
       </c>
@@ -6346,7 +6368,7 @@
       </c>
       <c r="I116" s="5"/>
     </row>
-    <row r="117" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" ht="29.25">
       <c r="A117" s="10" t="s">
         <v>39</v>
       </c>
@@ -6373,7 +6395,7 @@
       </c>
       <c r="I117" s="5"/>
     </row>
-    <row r="118" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" ht="29.25">
       <c r="A118" s="10" t="s">
         <v>39</v>
       </c>
@@ -6400,7 +6422,7 @@
       </c>
       <c r="I118" s="5"/>
     </row>
-    <row r="119" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" ht="29.25">
       <c r="A119" s="10" t="s">
         <v>39</v>
       </c>
@@ -6427,7 +6449,7 @@
       </c>
       <c r="I119" s="5"/>
     </row>
-    <row r="120" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" ht="29.25">
       <c r="A120" s="10" t="s">
         <v>39</v>
       </c>
@@ -6454,7 +6476,7 @@
       </c>
       <c r="I120" s="5"/>
     </row>
-    <row r="121" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" ht="29.25">
       <c r="A121" s="10" t="s">
         <v>39</v>
       </c>
@@ -6481,7 +6503,7 @@
       </c>
       <c r="I121" s="5"/>
     </row>
-    <row r="122" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" ht="29.25">
       <c r="A122" s="10" t="s">
         <v>39</v>
       </c>
@@ -6508,7 +6530,7 @@
       </c>
       <c r="I122" s="5"/>
     </row>
-    <row r="123" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" ht="29.25">
       <c r="A123" s="10" t="s">
         <v>39</v>
       </c>
@@ -6535,7 +6557,7 @@
       </c>
       <c r="I123" s="5"/>
     </row>
-    <row r="124" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" ht="29.25">
       <c r="A124" s="10" t="s">
         <v>39</v>
       </c>
@@ -6562,7 +6584,7 @@
       </c>
       <c r="I124" s="5"/>
     </row>
-    <row r="125" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" ht="29.25">
       <c r="A125" s="10" t="s">
         <v>39</v>
       </c>
@@ -6589,7 +6611,7 @@
       </c>
       <c r="I125" s="5"/>
     </row>
-    <row r="126" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" ht="29.25">
       <c r="A126" s="10" t="s">
         <v>39</v>
       </c>
@@ -6616,7 +6638,7 @@
       </c>
       <c r="I126" s="5"/>
     </row>
-    <row r="127" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" ht="29.25">
       <c r="A127" s="10" t="s">
         <v>39</v>
       </c>
@@ -6643,7 +6665,7 @@
       </c>
       <c r="I127" s="5"/>
     </row>
-    <row r="128" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" ht="29.25">
       <c r="A128" s="10" t="s">
         <v>39</v>
       </c>
@@ -6670,7 +6692,7 @@
       </c>
       <c r="I128" s="5"/>
     </row>
-    <row r="129" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" ht="29.25">
       <c r="A129" s="10" t="s">
         <v>39</v>
       </c>
@@ -6697,7 +6719,7 @@
       </c>
       <c r="I129" s="5"/>
     </row>
-    <row r="130" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" ht="29.25">
       <c r="A130" s="10" t="s">
         <v>39</v>
       </c>
@@ -6724,7 +6746,7 @@
       </c>
       <c r="I130" s="5"/>
     </row>
-    <row r="131" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:9" ht="29.25">
       <c r="A131" s="10" t="s">
         <v>39</v>
       </c>
@@ -6751,7 +6773,7 @@
       </c>
       <c r="I131" s="5"/>
     </row>
-    <row r="132" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" ht="29.25">
       <c r="A132" s="10" t="s">
         <v>39</v>
       </c>
@@ -6778,7 +6800,7 @@
       </c>
       <c r="I132" s="5"/>
     </row>
-    <row r="133" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9" ht="29.25">
       <c r="A133" s="10" t="s">
         <v>39</v>
       </c>
@@ -6805,7 +6827,7 @@
       </c>
       <c r="I133" s="5"/>
     </row>
-    <row r="134" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9" ht="29.25">
       <c r="A134" s="10" t="s">
         <v>39</v>
       </c>
@@ -6832,7 +6854,7 @@
       </c>
       <c r="I134" s="5"/>
     </row>
-    <row r="135" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:9" ht="29.25">
       <c r="A135" s="10" t="s">
         <v>39</v>
       </c>
@@ -6859,7 +6881,7 @@
       </c>
       <c r="I135" s="5"/>
     </row>
-    <row r="136" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:9" ht="29.25">
       <c r="A136" s="10" t="s">
         <v>39</v>
       </c>
@@ -6886,7 +6908,7 @@
       </c>
       <c r="I136" s="5"/>
     </row>
-    <row r="137" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9" ht="43.5">
       <c r="A137" s="10" t="s">
         <v>39</v>
       </c>
@@ -6913,7 +6935,7 @@
       </c>
       <c r="I137" s="5"/>
     </row>
-    <row r="138" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9" ht="43.5">
       <c r="A138" s="10" t="s">
         <v>39</v>
       </c>
@@ -6940,7 +6962,7 @@
       </c>
       <c r="I138" s="5"/>
     </row>
-    <row r="139" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:9" ht="43.5">
       <c r="A139" s="10" t="s">
         <v>39</v>
       </c>
@@ -6967,7 +6989,7 @@
       </c>
       <c r="I139" s="5"/>
     </row>
-    <row r="140" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:9" ht="43.5">
       <c r="A140" s="10" t="s">
         <v>39</v>
       </c>
@@ -6994,7 +7016,7 @@
       </c>
       <c r="I140" s="5"/>
     </row>
-    <row r="141" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:9" ht="29.25">
       <c r="A141" s="10" t="s">
         <v>39</v>
       </c>
@@ -7021,7 +7043,7 @@
       </c>
       <c r="I141" s="5"/>
     </row>
-    <row r="142" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:9" ht="28.5">
       <c r="A142" s="10" t="s">
         <v>39</v>
       </c>
@@ -7048,7 +7070,7 @@
       </c>
       <c r="I142" s="5"/>
     </row>
-    <row r="143" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:9" ht="44.25">
       <c r="A143" s="10" t="s">
         <v>39</v>
       </c>
@@ -7075,7 +7097,7 @@
       </c>
       <c r="I143" s="5"/>
     </row>
-    <row r="144" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:9" ht="44.25">
       <c r="A144" s="10" t="s">
         <v>39</v>
       </c>
@@ -7102,7 +7124,7 @@
       </c>
       <c r="I144" s="5"/>
     </row>
-    <row r="145" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" ht="58.5">
       <c r="A145" s="10" t="s">
         <v>39</v>
       </c>
@@ -7129,7 +7151,7 @@
       </c>
       <c r="I145" s="5"/>
     </row>
-    <row r="146" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" ht="58.5">
       <c r="A146" s="10" t="s">
         <v>39</v>
       </c>
@@ -7156,7 +7178,7 @@
       </c>
       <c r="I146" s="5"/>
     </row>
-    <row r="147" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" ht="58.5">
       <c r="A147" s="10" t="s">
         <v>39</v>
       </c>
@@ -7183,7 +7205,7 @@
       </c>
       <c r="I147" s="5"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9">
       <c r="A148" s="5"/>
       <c r="B148" s="6"/>
       <c r="C148" s="6"/>
@@ -7194,7 +7216,7 @@
       <c r="H148" s="5"/>
       <c r="I148" s="5"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9">
       <c r="A149" s="5"/>
       <c r="B149" s="6"/>
       <c r="C149" s="6"/>
@@ -7205,7 +7227,7 @@
       <c r="H149" s="5"/>
       <c r="I149" s="5"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9">
       <c r="A150" s="5"/>
       <c r="B150" s="6"/>
       <c r="C150" s="6"/>
@@ -7216,7 +7238,7 @@
       <c r="H150" s="5"/>
       <c r="I150" s="5"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9">
       <c r="A151" s="5"/>
       <c r="B151" s="6"/>
       <c r="C151" s="6"/>
@@ -7227,31 +7249,31 @@
       <c r="H151" s="5"/>
       <c r="I151" s="5"/>
     </row>
-    <row r="152" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="18" t="s">
+    <row r="152" spans="1:9" s="7" customFormat="1">
+      <c r="A152" s="19" t="s">
         <v>379</v>
       </c>
-      <c r="B152" s="18"/>
-      <c r="C152" s="18"/>
-      <c r="D152" s="18"/>
-      <c r="E152" s="18"/>
-      <c r="F152" s="18"/>
-      <c r="G152" s="18"/>
-      <c r="H152" s="18"/>
-      <c r="I152" s="18"/>
+      <c r="B152" s="19"/>
+      <c r="C152" s="19"/>
+      <c r="D152" s="19"/>
+      <c r="E152" s="19"/>
+      <c r="F152" s="19"/>
+      <c r="G152" s="19"/>
+      <c r="H152" s="19"/>
+      <c r="I152" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A152:I152"/>
   </mergeCells>
-  <conditionalFormatting sqref="E77:E83">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="silabs">
-      <formula>NOT(ISERROR(SEARCH("silabs",E77)))</formula>
+  <conditionalFormatting sqref="A2:H147">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TODO">
+      <formula>NOT(ISERROR(SEARCH("TODO",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:H147">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="TODO">
-      <formula>NOT(ISERROR(SEARCH("TODO",A2)))</formula>
+  <conditionalFormatting sqref="E77:E83">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="silabs">
+      <formula>NOT(ISERROR(SEARCH("silabs",E77)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -7259,7 +7281,7 @@
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{60D2BEE7-449C-4D98-B095-39D70AC3291D}">
           <x14:formula1>
             <xm:f>DONOTDELETE!$A$3:$A$27</xm:f>
@@ -7292,14 +7314,14 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="26.109375" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
@@ -7312,7 +7334,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -7323,7 +7345,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -7334,7 +7356,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -7345,7 +7367,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -7356,7 +7378,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -7367,7 +7389,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -7375,7 +7397,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -7383,7 +7405,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="C10" t="s">
         <v>23</v>
       </c>
@@ -7402,30 +7424,30 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="90.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="106.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="90.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="106.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B2" s="19" t="s">
+    <row r="2" spans="2:5">
+      <c r="B2" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5">
       <c r="B3" s="16" t="s">
         <v>30</v>
       </c>
@@ -7439,7 +7461,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5">
       <c r="B4" s="16" t="s">
         <v>369</v>
       </c>
@@ -7451,7 +7473,7 @@
       </c>
       <c r="E4" s="16"/>
     </row>
-    <row r="5" spans="2:5" ht="55.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" ht="57.75">
       <c r="B5" s="16" t="s">
         <v>39</v>
       </c>
@@ -7463,7 +7485,7 @@
       </c>
       <c r="E5" s="16"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5">
       <c r="B6" s="16" t="s">
         <v>58</v>
       </c>
@@ -7471,7 +7493,7 @@
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5">
       <c r="B7" s="16" t="s">
         <v>356</v>
       </c>
@@ -7485,7 +7507,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5">
       <c r="B8" s="16" t="s">
         <v>360</v>
       </c>
@@ -7499,7 +7521,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5">
       <c r="B9" s="16" t="s">
         <v>36</v>
       </c>
@@ -7511,7 +7533,7 @@
       </c>
       <c r="E9" s="16"/>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5">
       <c r="B10" s="16" t="s">
         <v>367</v>
       </c>

</xml_diff>

<commit_message>
add minhv_pma_block to vplan
Signed-off-by: Kristine Dosvik <krdosvik@silabs.com>
</commit_message>
<xml_diff>
--- a/cv32e40s/docs/VerifPlans/Simulation/interrupts/CV32E40SX_CLIC.xlsx
+++ b/cv32e40s/docs/VerifPlans/Simulation/interrupts/CV32E40SX_CLIC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\openhw\core-v-verif_40s\cv32e40s\docs\VerifPlans\Simulation\interrupts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krdosvik\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0700F57D-6730-46B3-A55F-7643D604952C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23298965-2AF0-4E21-8D02-CE9A7987F05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="High-level Feature" sheetId="1" r:id="rId1"/>
@@ -2897,7 +2897,7 @@
     <t>clic_cg.cp_lvl</t>
   </si>
   <si>
-    <t>clic::invalid_mtvt_ptr_exec_mret</t>
+    <t>clic::invalid_mtvt_ptr_exec_mret, minhv_pma_block.c</t>
   </si>
 </sst>
 </file>
@@ -3571,9 +3571,9 @@
   <dimension ref="A1:I152"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
+      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
added mepc minhv misalignement test
Signed-off-by: Kristine Dosvik <krdosvik@silabs.com>
</commit_message>
<xml_diff>
--- a/cv32e40s/docs/VerifPlans/Simulation/interrupts/CV32E40SX_CLIC.xlsx
+++ b/cv32e40s/docs/VerifPlans/Simulation/interrupts/CV32E40SX_CLIC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krdosvik\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23298965-2AF0-4E21-8D02-CE9A7987F05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75F93FB-3503-470C-99C7-2DB491E561D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
     Should this and all other assertion checks include assertion coverage?</t>
       </text>
     </comment>
-    <comment ref="B99" authorId="1" shapeId="0" xr:uid="{07A754E4-5049-4597-88FB-936DEA94A796}">
+    <comment ref="B100" authorId="1" shapeId="0" xr:uid="{07A754E4-5049-4597-88FB-936DEA94A796}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1377" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="464">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -2898,6 +2898,22 @@
   </si>
   <si>
     <t>clic::invalid_mtvt_ptr_exec_mret, minhv_pma_block.c</t>
+  </si>
+  <si>
+    <t>mret minhv=1</t>
+  </si>
+  <si>
+    <t>CLIC 0.9-draft 12/19/2023</t>
+  </si>
+  <si>
+    <t>DTC: clic :: mret_with_minhv
+clic ::mret_with_minhv_and_unaligned_mepc</t>
+  </si>
+  <si>
+    <t>Run mret when minhv is set. Check that the next instruction to be executed is the address pointed to by the mepc, and check that mepc gets naturally aligned to XLEN/8 byte.</t>
+  </si>
+  <si>
+    <t>"If the xinhv bit is set, the hart resumes the trap handler memory access to retrieve the function pointer for vectoring with permissions corresponding to the previous privilege mode. The trap handler function address is obtained from the current privilege mode’s xepc with the low bits of the address cleared to force the access to be naturally aligned to an XLEN/8-byte table entry."</t>
   </si>
 </sst>
 </file>
@@ -3554,13 +3570,13 @@
   <threadedComment ref="H18" dT="2021-09-09T14:23:41.65" personId="{710810F1-68FD-4BBA-B9D0-AA1628458E0A}" id="{7885884D-C7FD-41BA-8576-33EA399AE858}">
     <text>Should this and all other assertion checks include assertion coverage?</text>
   </threadedComment>
-  <threadedComment ref="B99" dT="2020-09-24T12:42:19.70" personId="{193092B7-7E1F-4488-B1DA-C3EB0981CF6E}" id="{07A754E4-5049-4597-88FB-936DEA94A796}" done="1">
+  <threadedComment ref="B100" dT="2020-09-24T12:42:19.70" personId="{193092B7-7E1F-4488-B1DA-C3EB0981CF6E}" id="{07A754E4-5049-4597-88FB-936DEA94A796}" done="1">
     <text>General comment for all the "Interrupt Instruction" features in this DV plan.  This is important and will produce a large, difficult to fill functional coverage model.  Is there a way to use FV to provide exhaustive coverage of this?</text>
   </threadedComment>
-  <threadedComment ref="B99" dT="2020-09-29T20:07:02.50" personId="{6EF99FC1-4767-4199-A11C-C305DAB2F1C1}" id="{070C2FA9-EF36-4F23-8066-54666C7B105F}" parentId="{07A754E4-5049-4597-88FB-936DEA94A796}">
+  <threadedComment ref="B100" dT="2020-09-29T20:07:02.50" personId="{6EF99FC1-4767-4199-A11C-C305DAB2F1C1}" id="{070C2FA9-EF36-4F23-8066-54666C7B105F}" parentId="{07A754E4-5049-4597-88FB-936DEA94A796}">
     <text>Coverage reports show all instructions covered here.</text>
   </threadedComment>
-  <threadedComment ref="B99" dT="2020-09-29T23:01:29.17" personId="{6EF99FC1-4767-4199-A11C-C305DAB2F1C1}" id="{AB040D79-0384-4884-9851-B375973FC3A2}" parentId="{07A754E4-5049-4597-88FB-936DEA94A796}">
+  <threadedComment ref="B100" dT="2020-09-29T23:01:29.17" personId="{6EF99FC1-4767-4199-A11C-C305DAB2F1C1}" id="{AB040D79-0384-4884-9851-B375973FC3A2}" parentId="{07A754E4-5049-4597-88FB-936DEA94A796}">
     <text>Will leave of functional coverage as defined here.</text>
   </threadedComment>
 </ThreadedComments>
@@ -3568,12 +3584,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I152"/>
+  <dimension ref="A1:I153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
+      <selection pane="bottomLeft" activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="15"/>
@@ -4952,7 +4968,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="255" customHeight="1">
+    <row r="48" spans="1:9" ht="267.75" customHeight="1">
       <c r="A48" s="10" t="s">
         <v>36</v>
       </c>
@@ -5706,65 +5722,65 @@
         <v>380</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="71.25">
-      <c r="A74" s="24" t="s">
+    <row r="74" spans="1:9" ht="114">
+      <c r="A74" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="B74" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="C74" s="11" t="s">
+        <v>459</v>
+      </c>
+      <c r="D74" s="11" t="s">
+        <v>463</v>
+      </c>
+      <c r="E74" s="11" t="s">
+        <v>462</v>
+      </c>
+      <c r="F74" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G74" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H74" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I74" s="21" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="71.25">
+      <c r="A75" s="24" t="s">
         <v>368</v>
       </c>
-      <c r="B74" s="25" t="s">
+      <c r="B75" s="25" t="s">
         <v>374</v>
       </c>
-      <c r="C74" s="25" t="s">
+      <c r="C75" s="25" t="s">
         <v>375</v>
       </c>
-      <c r="D74" s="25" t="s">
+      <c r="D75" s="25" t="s">
         <v>373</v>
       </c>
-      <c r="E74" s="25" t="s">
+      <c r="E75" s="25" t="s">
         <v>376</v>
       </c>
-      <c r="F74" s="25" t="s">
+      <c r="F75" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="G74" s="25" t="s">
+      <c r="G75" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="H74" s="25" t="s">
+      <c r="H75" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="I74" s="23" t="s">
+      <c r="I75" s="23" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="114">
-      <c r="A75" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B75" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="C75" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="D75" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="E75" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="F75" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G75" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H75" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="I75" s="5" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="128.25">
+    <row r="76" spans="1:9" ht="114">
       <c r="A76" s="10" t="s">
         <v>30</v>
       </c>
@@ -5775,10 +5791,10 @@
         <v>228</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F76" s="11" t="s">
         <v>15</v>
@@ -5793,7 +5809,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="114">
+    <row r="77" spans="1:9" ht="128.25">
       <c r="A77" s="10" t="s">
         <v>30</v>
       </c>
@@ -5803,26 +5819,26 @@
       <c r="C77" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="D77" s="13" t="s">
-        <v>233</v>
+      <c r="D77" s="11" t="s">
+        <v>231</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>213</v>
+        <v>232</v>
       </c>
       <c r="F77" s="11" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="G77" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H77" s="11" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="I77" s="5" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="28.5">
+    <row r="78" spans="1:9" ht="114">
       <c r="A78" s="10" t="s">
         <v>30</v>
       </c>
@@ -5833,39 +5849,39 @@
         <v>228</v>
       </c>
       <c r="D78" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="E78" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="F78" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G78" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H78" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I78" s="5" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="28.5">
+      <c r="A79" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B79" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="C79" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="D79" s="13" t="s">
         <v>234</v>
       </c>
-      <c r="E78" s="11" t="s">
+      <c r="E79" s="11" t="s">
         <v>235</v>
-      </c>
-      <c r="F78" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G78" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="H78" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="I78" s="5" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" ht="29.25">
-      <c r="A79" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B79" s="14" t="s">
-        <v>236</v>
-      </c>
-      <c r="C79" s="14" t="s">
-        <v>237</v>
-      </c>
-      <c r="D79" s="14" t="s">
-        <v>238</v>
-      </c>
-      <c r="E79" s="14" t="s">
-        <v>239</v>
       </c>
       <c r="F79" s="11" t="s">
         <v>18</v>
@@ -5877,10 +5893,10 @@
         <v>14</v>
       </c>
       <c r="I79" s="5" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" ht="28.5">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="29.25">
       <c r="A80" s="10" t="s">
         <v>36</v>
       </c>
@@ -5888,13 +5904,13 @@
         <v>236</v>
       </c>
       <c r="C80" s="14" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D80" s="14" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E80" s="14" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="F80" s="11" t="s">
         <v>18</v>
@@ -5906,10 +5922,10 @@
         <v>14</v>
       </c>
       <c r="I80" s="5" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" ht="29.25">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="28.5">
       <c r="A81" s="10" t="s">
         <v>36</v>
       </c>
@@ -5917,13 +5933,13 @@
         <v>236</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D81" s="14" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E81" s="14" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F81" s="11" t="s">
         <v>18</v>
@@ -5935,24 +5951,24 @@
         <v>14</v>
       </c>
       <c r="I81" s="5" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" ht="42.75">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="29.25">
       <c r="A82" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B82" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="C82" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="D82" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="E82" s="11" t="s">
-        <v>249</v>
+        <v>36</v>
+      </c>
+      <c r="B82" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="C82" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="D82" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="E82" s="14" t="s">
+        <v>245</v>
       </c>
       <c r="F82" s="11" t="s">
         <v>18</v>
@@ -5964,10 +5980,10 @@
         <v>14</v>
       </c>
       <c r="I82" s="5" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" ht="57.75">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="42.75">
       <c r="A83" s="10" t="s">
         <v>30</v>
       </c>
@@ -5975,13 +5991,13 @@
         <v>246</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F83" s="11" t="s">
         <v>18</v>
@@ -5993,39 +6009,39 @@
         <v>14</v>
       </c>
       <c r="I83" s="5" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="57.75">
+      <c r="A84" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B84" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="C84" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="E84" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="F84" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G84" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H84" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I84" s="5" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="71.25">
-      <c r="A84" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B84" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="C84" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="D84" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="E84" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="F84" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G84" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H84" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="I84" s="21" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" ht="114.75">
+    <row r="85" spans="1:9" ht="71.25">
       <c r="A85" s="10" t="s">
         <v>36</v>
       </c>
@@ -6033,13 +6049,13 @@
         <v>253</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E85" s="11" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F85" s="11" t="s">
         <v>15</v>
@@ -6050,11 +6066,11 @@
       <c r="H85" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I85" s="23" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" ht="199.5">
+      <c r="I85" s="21" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="114.75">
       <c r="A86" s="10" t="s">
         <v>36</v>
       </c>
@@ -6062,13 +6078,13 @@
         <v>253</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E86" s="11" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F86" s="11" t="s">
         <v>15</v>
@@ -6080,7 +6096,7 @@
         <v>14</v>
       </c>
       <c r="I86" s="23" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="199.5">
@@ -6091,13 +6107,13 @@
         <v>253</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D87" s="11" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="E87" s="11" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F87" s="11" t="s">
         <v>15</v>
@@ -6112,7 +6128,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="171">
+    <row r="88" spans="1:9" ht="199.5">
       <c r="A88" s="10" t="s">
         <v>36</v>
       </c>
@@ -6120,13 +6136,13 @@
         <v>253</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F88" s="11" t="s">
         <v>15</v>
@@ -6141,7 +6157,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="114">
+    <row r="89" spans="1:9" ht="171">
       <c r="A89" s="10" t="s">
         <v>36</v>
       </c>
@@ -6149,13 +6165,13 @@
         <v>253</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E89" s="11" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F89" s="11" t="s">
         <v>15</v>
@@ -6170,7 +6186,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="142.5">
+    <row r="90" spans="1:9" ht="114">
       <c r="A90" s="10" t="s">
         <v>36</v>
       </c>
@@ -6178,13 +6194,13 @@
         <v>253</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E90" s="11" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F90" s="11" t="s">
         <v>15</v>
@@ -6199,7 +6215,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="156.75">
+    <row r="91" spans="1:9" ht="142.5">
       <c r="A91" s="10" t="s">
         <v>36</v>
       </c>
@@ -6207,13 +6223,13 @@
         <v>253</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E91" s="11" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F91" s="11" t="s">
         <v>15</v>
@@ -6228,7 +6244,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="128.25">
+    <row r="92" spans="1:9" ht="156.75">
       <c r="A92" s="10" t="s">
         <v>36</v>
       </c>
@@ -6236,13 +6252,13 @@
         <v>253</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="E92" s="11" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F92" s="11" t="s">
         <v>15</v>
@@ -6257,7 +6273,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="199.5">
+    <row r="93" spans="1:9" ht="128.25">
       <c r="A93" s="10" t="s">
         <v>36</v>
       </c>
@@ -6265,13 +6281,13 @@
         <v>253</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E93" s="11" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F93" s="11" t="s">
         <v>15</v>
@@ -6294,13 +6310,13 @@
         <v>253</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D94" s="11" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E94" s="11" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F94" s="11" t="s">
         <v>15</v>
@@ -6315,7 +6331,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="142.5">
+    <row r="95" spans="1:9" ht="199.5">
       <c r="A95" s="10" t="s">
         <v>36</v>
       </c>
@@ -6323,13 +6339,13 @@
         <v>253</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="E95" s="11" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="F95" s="11" t="s">
         <v>15</v>
@@ -6344,7 +6360,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="128.25">
+    <row r="96" spans="1:9" ht="142.5">
       <c r="A96" s="10" t="s">
         <v>36</v>
       </c>
@@ -6352,13 +6368,13 @@
         <v>253</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D96" s="11" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="E96" s="11" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F96" s="11" t="s">
         <v>15</v>
@@ -6373,7 +6389,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="142.5">
+    <row r="97" spans="1:9" ht="128.25">
       <c r="A97" s="10" t="s">
         <v>36</v>
       </c>
@@ -6381,13 +6397,13 @@
         <v>253</v>
       </c>
       <c r="C97" s="11" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E97" s="11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F97" s="11" t="s">
         <v>15</v>
@@ -6402,7 +6418,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="185.25">
+    <row r="98" spans="1:9" ht="142.5">
       <c r="A98" s="10" t="s">
         <v>36</v>
       </c>
@@ -6410,13 +6426,13 @@
         <v>253</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D98" s="11" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E98" s="11" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="F98" s="11" t="s">
         <v>15</v>
@@ -6431,21 +6447,21 @@
         <v>455</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="29.25">
+    <row r="99" spans="1:9" ht="185.25">
       <c r="A99" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B99" s="11" t="s">
-        <v>217</v>
+        <v>253</v>
       </c>
       <c r="C99" s="11" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D99" s="11" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E99" s="11" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F99" s="11" t="s">
         <v>15</v>
@@ -6456,8 +6472,8 @@
       <c r="H99" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I99" s="21" t="s">
-        <v>440</v>
+      <c r="I99" s="23" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="29.25">
@@ -6468,7 +6484,7 @@
         <v>217</v>
       </c>
       <c r="C100" s="11" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D100" s="11" t="s">
         <v>300</v>
@@ -6497,7 +6513,7 @@
         <v>217</v>
       </c>
       <c r="C101" s="11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D101" s="11" t="s">
         <v>300</v>
@@ -6526,7 +6542,7 @@
         <v>217</v>
       </c>
       <c r="C102" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D102" s="11" t="s">
         <v>300</v>
@@ -6555,7 +6571,7 @@
         <v>217</v>
       </c>
       <c r="C103" s="11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D103" s="11" t="s">
         <v>300</v>
@@ -6584,7 +6600,7 @@
         <v>217</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D104" s="11" t="s">
         <v>300</v>
@@ -6613,7 +6629,7 @@
         <v>217</v>
       </c>
       <c r="C105" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D105" s="11" t="s">
         <v>300</v>
@@ -6634,7 +6650,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="57.75">
+    <row r="106" spans="1:9" ht="29.25">
       <c r="A106" s="10" t="s">
         <v>39</v>
       </c>
@@ -6642,7 +6658,7 @@
         <v>217</v>
       </c>
       <c r="C106" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D106" s="11" t="s">
         <v>300</v>
@@ -6660,10 +6676,10 @@
         <v>14</v>
       </c>
       <c r="I106" s="21" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" ht="29.25">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="57.75">
       <c r="A107" s="10" t="s">
         <v>39</v>
       </c>
@@ -6671,7 +6687,7 @@
         <v>217</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D107" s="11" t="s">
         <v>300</v>
@@ -6688,8 +6704,8 @@
       <c r="H107" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I107" s="23" t="s">
-        <v>454</v>
+      <c r="I107" s="21" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="108" spans="1:9" ht="29.25">
@@ -6700,7 +6716,7 @@
         <v>217</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D108" s="11" t="s">
         <v>300</v>
@@ -6729,7 +6745,7 @@
         <v>217</v>
       </c>
       <c r="C109" s="11" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D109" s="11" t="s">
         <v>300</v>
@@ -6758,7 +6774,7 @@
         <v>217</v>
       </c>
       <c r="C110" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D110" s="11" t="s">
         <v>300</v>
@@ -6787,7 +6803,7 @@
         <v>217</v>
       </c>
       <c r="C111" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D111" s="11" t="s">
         <v>300</v>
@@ -6816,7 +6832,7 @@
         <v>217</v>
       </c>
       <c r="C112" s="11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D112" s="11" t="s">
         <v>300</v>
@@ -6845,7 +6861,7 @@
         <v>217</v>
       </c>
       <c r="C113" s="11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D113" s="11" t="s">
         <v>300</v>
@@ -6874,7 +6890,7 @@
         <v>217</v>
       </c>
       <c r="C114" s="11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D114" s="11" t="s">
         <v>300</v>
@@ -6903,7 +6919,7 @@
         <v>217</v>
       </c>
       <c r="C115" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D115" s="11" t="s">
         <v>300</v>
@@ -6932,7 +6948,7 @@
         <v>217</v>
       </c>
       <c r="C116" s="11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D116" s="11" t="s">
         <v>300</v>
@@ -6961,7 +6977,7 @@
         <v>217</v>
       </c>
       <c r="C117" s="11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D117" s="11" t="s">
         <v>300</v>
@@ -6990,7 +7006,7 @@
         <v>217</v>
       </c>
       <c r="C118" s="11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D118" s="11" t="s">
         <v>300</v>
@@ -7011,7 +7027,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="57.75">
+    <row r="119" spans="1:9" ht="29.25">
       <c r="A119" s="10" t="s">
         <v>39</v>
       </c>
@@ -7019,7 +7035,7 @@
         <v>217</v>
       </c>
       <c r="C119" s="11" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D119" s="11" t="s">
         <v>300</v>
@@ -7036,11 +7052,11 @@
       <c r="H119" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I119" s="21" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" ht="29.25">
+      <c r="I119" s="23" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" ht="57.75">
       <c r="A120" s="10" t="s">
         <v>39</v>
       </c>
@@ -7048,7 +7064,7 @@
         <v>217</v>
       </c>
       <c r="C120" s="11" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D120" s="11" t="s">
         <v>300</v>
@@ -7066,10 +7082,10 @@
         <v>14</v>
       </c>
       <c r="I120" s="21" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" ht="57.75">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" ht="29.25">
       <c r="A121" s="10" t="s">
         <v>39</v>
       </c>
@@ -7077,7 +7093,7 @@
         <v>217</v>
       </c>
       <c r="C121" s="11" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D121" s="11" t="s">
         <v>300</v>
@@ -7095,10 +7111,10 @@
         <v>14</v>
       </c>
       <c r="I121" s="21" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" ht="29.25">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" ht="57.75">
       <c r="A122" s="10" t="s">
         <v>39</v>
       </c>
@@ -7106,7 +7122,7 @@
         <v>217</v>
       </c>
       <c r="C122" s="11" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D122" s="11" t="s">
         <v>300</v>
@@ -7124,7 +7140,7 @@
         <v>14</v>
       </c>
       <c r="I122" s="21" t="s">
-        <v>440</v>
+        <v>447</v>
       </c>
     </row>
     <row r="123" spans="1:9" ht="29.25">
@@ -7135,7 +7151,7 @@
         <v>217</v>
       </c>
       <c r="C123" s="11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D123" s="11" t="s">
         <v>300</v>
@@ -7164,7 +7180,7 @@
         <v>217</v>
       </c>
       <c r="C124" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D124" s="11" t="s">
         <v>300</v>
@@ -7193,7 +7209,7 @@
         <v>217</v>
       </c>
       <c r="C125" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D125" s="11" t="s">
         <v>300</v>
@@ -7210,8 +7226,8 @@
       <c r="H125" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I125" s="23" t="s">
-        <v>454</v>
+      <c r="I125" s="21" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="126" spans="1:9" ht="29.25">
@@ -7222,7 +7238,7 @@
         <v>217</v>
       </c>
       <c r="C126" s="11" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D126" s="11" t="s">
         <v>300</v>
@@ -7251,7 +7267,7 @@
         <v>217</v>
       </c>
       <c r="C127" s="11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D127" s="11" t="s">
         <v>300</v>
@@ -7280,7 +7296,7 @@
         <v>217</v>
       </c>
       <c r="C128" s="11" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D128" s="11" t="s">
         <v>300</v>
@@ -7309,7 +7325,7 @@
         <v>217</v>
       </c>
       <c r="C129" s="11" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D129" s="11" t="s">
         <v>300</v>
@@ -7326,8 +7342,8 @@
       <c r="H129" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I129" s="21" t="s">
-        <v>440</v>
+      <c r="I129" s="23" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="29.25">
@@ -7338,7 +7354,7 @@
         <v>217</v>
       </c>
       <c r="C130" s="11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D130" s="11" t="s">
         <v>300</v>
@@ -7367,7 +7383,7 @@
         <v>217</v>
       </c>
       <c r="C131" s="11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D131" s="11" t="s">
         <v>300</v>
@@ -7396,7 +7412,7 @@
         <v>217</v>
       </c>
       <c r="C132" s="11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D132" s="11" t="s">
         <v>300</v>
@@ -7425,7 +7441,7 @@
         <v>217</v>
       </c>
       <c r="C133" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D133" s="11" t="s">
         <v>300</v>
@@ -7446,7 +7462,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="134" spans="1:9" ht="57.75">
+    <row r="134" spans="1:9" ht="29.25">
       <c r="A134" s="10" t="s">
         <v>39</v>
       </c>
@@ -7454,7 +7470,7 @@
         <v>217</v>
       </c>
       <c r="C134" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D134" s="11" t="s">
         <v>300</v>
@@ -7472,10 +7488,10 @@
         <v>14</v>
       </c>
       <c r="I134" s="21" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" ht="29.25">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" ht="57.75">
       <c r="A135" s="10" t="s">
         <v>39</v>
       </c>
@@ -7483,7 +7499,7 @@
         <v>217</v>
       </c>
       <c r="C135" s="11" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D135" s="11" t="s">
         <v>300</v>
@@ -7501,10 +7517,10 @@
         <v>14</v>
       </c>
       <c r="I135" s="21" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9" ht="57.75">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" ht="29.25">
       <c r="A136" s="10" t="s">
         <v>39</v>
       </c>
@@ -7512,7 +7528,7 @@
         <v>217</v>
       </c>
       <c r="C136" s="11" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D136" s="11" t="s">
         <v>300</v>
@@ -7530,10 +7546,10 @@
         <v>14</v>
       </c>
       <c r="I136" s="21" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9" ht="43.5">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" ht="57.75">
       <c r="A137" s="10" t="s">
         <v>39</v>
       </c>
@@ -7541,7 +7557,7 @@
         <v>217</v>
       </c>
       <c r="C137" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D137" s="11" t="s">
         <v>300</v>
@@ -7558,8 +7574,8 @@
       <c r="H137" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I137" s="20" t="s">
-        <v>445</v>
+      <c r="I137" s="21" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="138" spans="1:9" ht="43.5">
@@ -7570,7 +7586,7 @@
         <v>217</v>
       </c>
       <c r="C138" s="11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D138" s="11" t="s">
         <v>300</v>
@@ -7599,7 +7615,7 @@
         <v>217</v>
       </c>
       <c r="C139" s="11" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D139" s="11" t="s">
         <v>300</v>
@@ -7628,7 +7644,7 @@
         <v>217</v>
       </c>
       <c r="C140" s="11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D140" s="11" t="s">
         <v>300</v>
@@ -7649,7 +7665,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="141" spans="1:9" ht="29.25">
+    <row r="141" spans="1:9" ht="43.5">
       <c r="A141" s="10" t="s">
         <v>39</v>
       </c>
@@ -7657,7 +7673,7 @@
         <v>217</v>
       </c>
       <c r="C141" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D141" s="11" t="s">
         <v>300</v>
@@ -7678,7 +7694,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="142" spans="1:9" ht="28.5">
+    <row r="142" spans="1:9" ht="29.25">
       <c r="A142" s="10" t="s">
         <v>39</v>
       </c>
@@ -7686,7 +7702,7 @@
         <v>217</v>
       </c>
       <c r="C142" s="11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D142" s="11" t="s">
         <v>300</v>
@@ -7703,11 +7719,11 @@
       <c r="H142" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I142" s="5" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="143" spans="1:9" ht="44.25">
+      <c r="I142" s="20" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" ht="28.5">
       <c r="A143" s="10" t="s">
         <v>39</v>
       </c>
@@ -7715,7 +7731,7 @@
         <v>217</v>
       </c>
       <c r="C143" s="11" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D143" s="11" t="s">
         <v>300</v>
@@ -7744,7 +7760,7 @@
         <v>217</v>
       </c>
       <c r="C144" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D144" s="11" t="s">
         <v>300</v>
@@ -7762,18 +7778,18 @@
         <v>14</v>
       </c>
       <c r="I144" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="145" spans="1:9" ht="58.5">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" ht="44.25">
       <c r="A145" s="10" t="s">
         <v>39</v>
       </c>
       <c r="B145" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="C145" s="15" t="s">
-        <v>347</v>
+      <c r="C145" s="11" t="s">
+        <v>346</v>
       </c>
       <c r="D145" s="11" t="s">
         <v>300</v>
@@ -7802,7 +7818,7 @@
         <v>217</v>
       </c>
       <c r="C146" s="15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D146" s="11" t="s">
         <v>300</v>
@@ -7831,7 +7847,7 @@
         <v>217</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D147" s="11" t="s">
         <v>300</v>
@@ -7852,16 +7868,34 @@
         <v>23</v>
       </c>
     </row>
-    <row r="148" spans="1:9">
-      <c r="A148" s="5"/>
-      <c r="B148" s="6"/>
-      <c r="C148" s="6"/>
-      <c r="D148" s="6"/>
-      <c r="E148" s="6"/>
-      <c r="F148" s="6"/>
-      <c r="G148" s="6"/>
-      <c r="H148" s="5"/>
-      <c r="I148" s="5"/>
+    <row r="148" spans="1:9" ht="58.5">
+      <c r="A148" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B148" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="C148" s="15" t="s">
+        <v>349</v>
+      </c>
+      <c r="D148" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="E148" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="F148" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G148" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H148" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I148" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="149" spans="1:9">
       <c r="A149" s="5"/>
@@ -7896,31 +7930,42 @@
       <c r="H151" s="5"/>
       <c r="I151" s="5"/>
     </row>
-    <row r="152" spans="1:9" s="7" customFormat="1">
-      <c r="A152" s="31" t="s">
+    <row r="152" spans="1:9">
+      <c r="A152" s="5"/>
+      <c r="B152" s="6"/>
+      <c r="C152" s="6"/>
+      <c r="D152" s="6"/>
+      <c r="E152" s="6"/>
+      <c r="F152" s="6"/>
+      <c r="G152" s="6"/>
+      <c r="H152" s="5"/>
+      <c r="I152" s="5"/>
+    </row>
+    <row r="153" spans="1:9" s="7" customFormat="1">
+      <c r="A153" s="31" t="s">
         <v>378</v>
       </c>
-      <c r="B152" s="31"/>
-      <c r="C152" s="31"/>
-      <c r="D152" s="31"/>
-      <c r="E152" s="31"/>
-      <c r="F152" s="31"/>
-      <c r="G152" s="31"/>
-      <c r="H152" s="31"/>
-      <c r="I152" s="31"/>
+      <c r="B153" s="31"/>
+      <c r="C153" s="31"/>
+      <c r="D153" s="31"/>
+      <c r="E153" s="31"/>
+      <c r="F153" s="31"/>
+      <c r="G153" s="31"/>
+      <c r="H153" s="31"/>
+      <c r="I153" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A152:I152"/>
+    <mergeCell ref="A153:I153"/>
   </mergeCells>
-  <conditionalFormatting sqref="A2:H147">
+  <conditionalFormatting sqref="A2:H148">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TODO">
       <formula>NOT(ISERROR(SEARCH("TODO",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E77:E83">
+  <conditionalFormatting sqref="E78:E84">
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="silabs">
-      <formula>NOT(ISERROR(SEARCH("silabs",E77)))</formula>
+      <formula>NOT(ISERROR(SEARCH("silabs",E78)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>